<commit_message>
Permenant: Remove Unneeded Texture
There was a texture in the permanent package that didn't exist anywhere and wasn't used by anything. It's also not default to any version of the game
</commit_message>
<xml_diff>
--- a/4. Menus/permanent/Power Models and Textures.xlsx
+++ b/4. Menus/permanent/Power Models and Textures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\XML2-Ultimate-Patch\4. Menus\permanent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15F18FF-BD01-4098-8AF1-8C4F288E67DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55E4B43-0800-41A5-86DF-79CA6A9E3233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="152">
   <si>
     <t>File</t>
   </si>
@@ -388,9 +388,6 @@
   </si>
   <si>
     <t>textures\gb_star.igb</t>
-  </si>
-  <si>
-    <t>textures\grnglow.igb</t>
   </si>
   <si>
     <t>textures\hit_ring.igb</t>
@@ -543,117 +540,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -784,26 +671,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -818,10 +685,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G123" totalsRowShown="0">
-  <autoFilter ref="A1:G123" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G123">
-    <sortCondition ref="A1:A123"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G122" totalsRowShown="0">
+  <autoFilter ref="A1:G122" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G122">
+    <sortCondition ref="A1:A122"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6B176F19-9C3E-4D2F-9828-AA9A0F4398C8}" name="File"/>
@@ -1119,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,12 +1045,12 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1201,12 +1068,12 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1224,7 +1091,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1247,12 +1114,12 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -1270,7 +1137,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1293,7 +1160,7 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1316,7 +1183,7 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1339,7 +1206,7 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1362,7 +1229,7 @@
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1385,7 +1252,7 @@
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1408,7 +1275,7 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1431,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1454,7 +1321,7 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1477,7 +1344,7 @@
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1500,7 +1367,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1523,7 +1390,7 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1546,12 +1413,12 @@
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -1569,7 +1436,7 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1592,7 +1459,7 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1615,12 +1482,12 @@
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
@@ -1638,7 +1505,7 @@
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1661,12 +1528,12 @@
         <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
@@ -1684,12 +1551,12 @@
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
@@ -1707,12 +1574,12 @@
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -1730,7 +1597,7 @@
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1753,7 +1620,7 @@
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1776,7 +1643,7 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1799,7 +1666,7 @@
         <v>18</v>
       </c>
       <c r="G29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1822,7 +1689,7 @@
         <v>21</v>
       </c>
       <c r="G30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1845,7 +1712,7 @@
         <v>21</v>
       </c>
       <c r="G31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1868,7 +1735,7 @@
         <v>21</v>
       </c>
       <c r="G32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1891,7 +1758,7 @@
         <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1914,7 +1781,7 @@
         <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1937,7 +1804,7 @@
         <v>18</v>
       </c>
       <c r="G35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1960,7 +1827,7 @@
         <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1983,7 +1850,7 @@
         <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2006,7 +1873,7 @@
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2029,7 +1896,7 @@
         <v>18</v>
       </c>
       <c r="G39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2052,7 +1919,7 @@
         <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2075,7 +1942,7 @@
         <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2098,7 +1965,7 @@
         <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2121,7 +1988,7 @@
         <v>15</v>
       </c>
       <c r="G43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2144,7 +2011,7 @@
         <v>15</v>
       </c>
       <c r="G44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2167,7 +2034,7 @@
         <v>15</v>
       </c>
       <c r="G45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2190,7 +2057,7 @@
         <v>15</v>
       </c>
       <c r="G46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2213,7 +2080,7 @@
         <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2236,7 +2103,7 @@
         <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2259,7 +2126,7 @@
         <v>15</v>
       </c>
       <c r="G49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2282,53 +2149,53 @@
         <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D51" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G51" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2336,19 +2203,19 @@
         <v>118</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
         <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G53" t="s">
         <v>149</v>
@@ -2356,48 +2223,48 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F54" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G54" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F55" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G55" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -2405,22 +2272,22 @@
         <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E56" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G56" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2428,50 +2295,50 @@
         <v>121</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D58" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E58" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G58" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
@@ -2489,12 +2356,12 @@
         <v>15</v>
       </c>
       <c r="G59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -2506,18 +2373,18 @@
         <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F60" t="s">
         <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
@@ -2529,18 +2396,18 @@
         <v>13</v>
       </c>
       <c r="E61" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F61" t="s">
         <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
@@ -2563,7 +2430,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
@@ -2581,12 +2448,12 @@
         <v>15</v>
       </c>
       <c r="G63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B64" t="s">
         <v>12</v>
@@ -2604,12 +2471,12 @@
         <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
         <v>12</v>
@@ -2627,12 +2494,12 @@
         <v>15</v>
       </c>
       <c r="G65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
@@ -2650,12 +2517,12 @@
         <v>15</v>
       </c>
       <c r="G66" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
@@ -2678,53 +2545,53 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D68" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
@@ -2742,12 +2609,12 @@
         <v>15</v>
       </c>
       <c r="G70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
@@ -2765,12 +2632,12 @@
         <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
@@ -2788,12 +2655,12 @@
         <v>15</v>
       </c>
       <c r="G72" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -2811,12 +2678,12 @@
         <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
         <v>12</v>
@@ -2839,7 +2706,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
@@ -2857,12 +2724,12 @@
         <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
@@ -2885,7 +2752,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
@@ -2903,12 +2770,12 @@
         <v>15</v>
       </c>
       <c r="G77" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
@@ -2926,12 +2793,12 @@
         <v>15</v>
       </c>
       <c r="G78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
@@ -2949,12 +2816,12 @@
         <v>15</v>
       </c>
       <c r="G79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B80" t="s">
         <v>12</v>
@@ -2972,12 +2839,12 @@
         <v>15</v>
       </c>
       <c r="G80" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
@@ -3000,7 +2867,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
         <v>12</v>
@@ -3018,12 +2885,12 @@
         <v>15</v>
       </c>
       <c r="G82" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
@@ -3041,12 +2908,12 @@
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
@@ -3064,30 +2931,30 @@
         <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D85" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E85" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F85" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G85" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3110,7 +2977,7 @@
         <v>21</v>
       </c>
       <c r="G86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3118,96 +2985,96 @@
         <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E87" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G87" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D88" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E88" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G88" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="B89" t="s">
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D89" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
       </c>
       <c r="F89" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G89" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B90" t="s">
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
       </c>
       <c r="F90" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G90" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B91" t="s">
         <v>12</v>
@@ -3225,27 +3092,27 @@
         <v>15</v>
       </c>
       <c r="G91" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="B92" t="s">
         <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D92" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E92" t="s">
         <v>14</v>
       </c>
       <c r="F92" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G92" t="s">
         <v>147</v>
@@ -3253,7 +3120,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="B93" t="s">
         <v>12</v>
@@ -3262,13 +3129,13 @@
         <v>20</v>
       </c>
       <c r="D93" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E93" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F93" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G93" t="s">
         <v>148</v>
@@ -3285,16 +3152,16 @@
         <v>20</v>
       </c>
       <c r="D94" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E94" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F94" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G94" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3302,50 +3169,50 @@
         <v>128</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C95" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D95" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E95" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G95" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D96" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E96" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F96" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G96" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B97" t="s">
         <v>12</v>
@@ -3363,104 +3230,104 @@
         <v>15</v>
       </c>
       <c r="G97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="B98" t="s">
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E98" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F98" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G98" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="B99" t="s">
         <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D99" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E99" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F99" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G99" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B100" t="s">
         <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D100" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E100" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F100" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G100" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="B101" t="s">
         <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D101" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E101" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G101" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="B102" t="s">
         <v>12</v>
@@ -3478,30 +3345,30 @@
         <v>15</v>
       </c>
       <c r="G102" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="B103" t="s">
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E103" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F103" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G103" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -3518,41 +3385,41 @@
         <v>20</v>
       </c>
       <c r="E104" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F104" t="s">
         <v>12</v>
       </c>
       <c r="G104" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="B105" t="s">
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D105" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E105" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F105" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G105" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
@@ -3564,18 +3431,18 @@
         <v>13</v>
       </c>
       <c r="E106" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F106" t="s">
         <v>15</v>
       </c>
       <c r="G106" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
@@ -3598,7 +3465,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
@@ -3616,127 +3483,127 @@
         <v>15</v>
       </c>
       <c r="G108" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="B109" t="s">
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D109" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E109" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F109" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G109" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D110" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E110" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F110" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G110" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B111" t="s">
         <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D111" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E111" t="s">
         <v>14</v>
       </c>
       <c r="F111" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G111" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B112" t="s">
         <v>12</v>
       </c>
       <c r="C112" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D112" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E112" t="s">
         <v>14</v>
       </c>
       <c r="F112" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G112" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="B113" t="s">
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D113" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
       </c>
       <c r="F113" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G113" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
@@ -3759,7 +3626,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="B115" t="s">
         <v>12</v>
@@ -3777,58 +3644,58 @@
         <v>15</v>
       </c>
       <c r="G115" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="B116" t="s">
         <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D116" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E116" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F116" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G116" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="B117" t="s">
         <v>12</v>
       </c>
       <c r="C117" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D117" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E117" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F117" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G117" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B118" t="s">
         <v>12</v>
@@ -3846,12 +3713,12 @@
         <v>15</v>
       </c>
       <c r="G118" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B119" t="s">
         <v>12</v>
@@ -3869,12 +3736,12 @@
         <v>15</v>
       </c>
       <c r="G119" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
@@ -3892,12 +3759,12 @@
         <v>15</v>
       </c>
       <c r="G120" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B121" t="s">
         <v>12</v>
@@ -3915,106 +3782,83 @@
         <v>15</v>
       </c>
       <c r="G121" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="B122" t="s">
         <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D122" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E122" t="s">
         <v>14</v>
       </c>
       <c r="F122" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G122" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>104</v>
-      </c>
-      <c r="B123" t="s">
-        <v>12</v>
-      </c>
-      <c r="C123" t="s">
-        <v>20</v>
-      </c>
-      <c r="D123" t="s">
-        <v>20</v>
-      </c>
-      <c r="E123" t="s">
-        <v>14</v>
-      </c>
-      <c r="F123" t="s">
-        <v>12</v>
-      </c>
-      <c r="G123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A123">
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
-    <cfRule type="notContainsText" dxfId="11" priority="15" operator="notContains" text=".igb">
-      <formula>ISERROR(SEARCH(".igb",A2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B123">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="notEqual">
+  <conditionalFormatting sqref="B2:B122">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="notEqual">
       <formula>"XML2 PC"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"XML2 PC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F123">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Custom">
+  <conditionalFormatting sqref="B2:F122">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Custom">
       <formula>NOT(ISERROR(SEARCH("Custom",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C123">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="notEqual">
+  <conditionalFormatting sqref="C2:C122">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="notEqual">
       <formula>"XML2 GameCube"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"XML2 GameCube"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D123">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="notEqual">
+  <conditionalFormatting sqref="D2:D122">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="notEqual">
       <formula>"XML2 PS2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"XML2 PS2"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E123">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
+  <conditionalFormatting sqref="E2:E122">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="notEqual">
       <formula>"XML2 PSP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"XML2 PSP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F123">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+  <conditionalFormatting sqref="F2:F122">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="notEqual">
       <formula>"XML2 Xbox"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"XML2 Xbox"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A122">
+    <cfRule type="duplicateValues" dxfId="1" priority="16"/>
+    <cfRule type="notContainsText" dxfId="0" priority="17" operator="notContains" text=".igb">
+      <formula>ISERROR(SEARCH(".igb",A2))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4028,13 +3872,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:F123</xm:sqref>
+          <xm:sqref>B2:F122</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2DF90B60-5089-44BA-BF59-8649B6D52DF3}">
           <x14:formula1>
             <xm:f>Sheet2!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G123</xm:sqref>
+          <xm:sqref>G2:G122</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4061,7 +3905,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4069,7 +3913,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -4077,7 +3921,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -4085,7 +3929,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -4093,7 +3937,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -4101,7 +3945,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -4109,7 +3953,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -4117,7 +3961,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -4125,7 +3969,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Permanent: Add Missing Files
Add missing files to the permanent package
</commit_message>
<xml_diff>
--- a/4. Menus/permanent/Power Models and Textures.xlsx
+++ b/4. Menus/permanent/Power Models and Textures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\XML2-Ultimate-Patch\4. Menus\permanent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D38DAA-D0DF-4387-A387-B79A3C9F7721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC944D3-BA08-4106-9280-170798D33C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="167">
   <si>
     <t>File</t>
   </si>
@@ -499,6 +499,45 @@
   </si>
   <si>
     <t>textures\spots.igb</t>
+  </si>
+  <si>
+    <t>models\chunks\met_8.igb</t>
+  </si>
+  <si>
+    <t>models\effects\fx_avalanche.igb</t>
+  </si>
+  <si>
+    <t>models\chunks\c_rocktunnel_c.igb</t>
+  </si>
+  <si>
+    <t>models\chunks\roc_3.igb</t>
+  </si>
+  <si>
+    <t>textures\chunks\stone_2.igb</t>
+  </si>
+  <si>
+    <t>textures\flame_base.igb</t>
+  </si>
+  <si>
+    <t>textures\s_waterwake.igb</t>
+  </si>
+  <si>
+    <t>textures\spots5.igb</t>
+  </si>
+  <si>
+    <t>textures\spray1.igb</t>
+  </si>
+  <si>
+    <t>textures\spray2.igb</t>
+  </si>
+  <si>
+    <t>textures\water_wash.igb</t>
+  </si>
+  <si>
+    <t>textures\whiteglow.igb</t>
+  </si>
+  <si>
+    <t>textures\whiteflash.igb</t>
   </si>
 </sst>
 </file>
@@ -546,7 +585,1567 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="182">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -821,10 +2420,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G124" totalsRowShown="0">
-  <autoFilter ref="A1:G124" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G124">
-    <sortCondition ref="G1:G124"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G137" totalsRowShown="0">
+  <autoFilter ref="A1:G137" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G137">
+    <sortCondition ref="A1:A137"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6B176F19-9C3E-4D2F-9828-AA9A0F4398C8}" name="File"/>
@@ -1122,10 +2721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G81" sqref="G81"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,7 +2785,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1198,18 +2797,18 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1227,12 +2826,12 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1250,12 +2849,12 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -1273,35 +2872,35 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -1324,7 +2923,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -1342,12 +2941,12 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -1365,12 +2964,12 @@
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1388,12 +2987,12 @@
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -1411,12 +3010,12 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -1434,12 +3033,12 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -1457,12 +3056,12 @@
         <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -1485,7 +3084,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1503,81 +3102,81 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
@@ -1595,12 +3194,12 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
@@ -1623,30 +3222,30 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
@@ -1664,12 +3263,12 @@
         <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
@@ -1687,12 +3286,12 @@
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
@@ -1710,12 +3309,12 @@
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -1733,12 +3332,12 @@
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -1756,12 +3355,12 @@
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -1779,12 +3378,12 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
@@ -1807,7 +3406,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -1830,7 +3429,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
@@ -1853,7 +3452,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -1876,7 +3475,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -1899,7 +3498,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -1917,104 +3516,104 @@
         <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G35" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G37" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G38" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
@@ -2032,12 +3631,12 @@
         <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
@@ -2060,53 +3659,53 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
@@ -2129,7 +3728,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
@@ -2152,53 +3751,53 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G46" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
@@ -2216,12 +3815,12 @@
         <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -2244,7 +3843,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
@@ -2267,7 +3866,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
@@ -2290,7 +3889,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
@@ -2302,18 +3901,18 @@
         <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
       </c>
       <c r="G51" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -2336,7 +3935,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
@@ -2359,7 +3958,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2382,30 +3981,30 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
@@ -2417,18 +4016,18 @@
         <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
       </c>
       <c r="G56" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
@@ -2451,7 +4050,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B58" t="s">
         <v>12</v>
@@ -2474,53 +4073,53 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F60" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G60" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
@@ -2538,81 +4137,81 @@
         <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F63" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G63" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="B64" t="s">
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G64" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="B65" t="s">
         <v>12</v>
@@ -2630,12 +4229,12 @@
         <v>15</v>
       </c>
       <c r="G65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
@@ -2653,12 +4252,12 @@
         <v>15</v>
       </c>
       <c r="G66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
@@ -2670,18 +4269,18 @@
         <v>13</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F67" t="s">
         <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
@@ -2699,12 +4298,12 @@
         <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
@@ -2727,7 +4326,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
@@ -2750,7 +4349,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
@@ -2773,7 +4372,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
@@ -2796,7 +4395,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -2814,12 +4413,12 @@
         <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="B74" t="s">
         <v>12</v>
@@ -2842,30 +4441,30 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E75" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G75" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
@@ -2888,7 +4487,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
@@ -2911,7 +4510,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
@@ -2929,12 +4528,12 @@
         <v>15</v>
       </c>
       <c r="G78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
@@ -2952,12 +4551,12 @@
         <v>15</v>
       </c>
       <c r="G79" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B80" t="s">
         <v>12</v>
@@ -2969,18 +4568,18 @@
         <v>13</v>
       </c>
       <c r="E80" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F80" t="s">
         <v>15</v>
       </c>
       <c r="G80" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
@@ -2992,18 +4591,18 @@
         <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F81" t="s">
         <v>15</v>
       </c>
       <c r="G81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B82" t="s">
         <v>12</v>
@@ -3015,18 +4614,18 @@
         <v>13</v>
       </c>
       <c r="E82" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F82" t="s">
         <v>15</v>
       </c>
       <c r="G82" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
@@ -3038,18 +4637,18 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F83" t="s">
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
@@ -3067,12 +4666,12 @@
         <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
         <v>12</v>
@@ -3090,12 +4689,12 @@
         <v>15</v>
       </c>
       <c r="G85" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B86" t="s">
         <v>12</v>
@@ -3113,12 +4712,12 @@
         <v>15</v>
       </c>
       <c r="G86" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B87" t="s">
         <v>12</v>
@@ -3136,12 +4735,12 @@
         <v>15</v>
       </c>
       <c r="G87" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B88" t="s">
         <v>12</v>
@@ -3159,127 +4758,127 @@
         <v>15</v>
       </c>
       <c r="G88" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B89" t="s">
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D89" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
       </c>
       <c r="F89" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G89" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
       </c>
       <c r="F90" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G90" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="B91" t="s">
         <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D91" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E91" t="s">
         <v>14</v>
       </c>
       <c r="F91" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E92" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F92" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G92" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D93" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E93" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F93" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G93" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="B94" t="s">
         <v>12</v>
@@ -3291,148 +4890,148 @@
         <v>20</v>
       </c>
       <c r="E94" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F94" t="s">
         <v>12</v>
       </c>
       <c r="G94" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B95" t="s">
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D95" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E95" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F95" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G95" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D96" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E96" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F96" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G96" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="B97" t="s">
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E97" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F97" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G97" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="B98" t="s">
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D98" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E98" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F98" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G98" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B99" t="s">
         <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D99" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E99" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F99" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G99" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B100" t="s">
         <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D100" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E100" t="s">
         <v>17</v>
       </c>
       <c r="F100" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G100" t="s">
         <v>148</v>
@@ -3440,7 +5039,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B101" t="s">
         <v>12</v>
@@ -3463,99 +5062,99 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="B102" t="s">
         <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D102" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E102" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F102" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G102" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B103" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D103" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E103" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F103" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G103" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
       <c r="B104" t="s">
         <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D104" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E104" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F104" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G104" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="B105" t="s">
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D105" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E105" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F105" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G105" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
@@ -3567,7 +5166,7 @@
         <v>20</v>
       </c>
       <c r="E106" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F106" t="s">
         <v>12</v>
@@ -3578,30 +5177,30 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D107" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E107" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F107" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G107" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
@@ -3624,48 +5223,48 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="B109" t="s">
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D109" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E109" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F109" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G109" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E110" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F110" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G110" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -3716,330 +5315,629 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="B113" t="s">
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D113" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E113" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F113" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G113" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D114" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E114" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F114" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G114" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="B115" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C115" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D115" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E115" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F115" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G115" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="B116" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D116" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E116" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F116" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G116" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C117" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D117" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E117" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F117" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G117" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>109</v>
+        <v>161</v>
       </c>
       <c r="B118" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D118" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E118" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F118" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G118" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="B119" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C119" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D119" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E119" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F119" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G119" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="B120" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C120" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D120" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E120" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F120" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G120" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E121" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F121" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G121" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B122" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D122" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E122" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F122" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G122" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B123" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D123" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E123" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F123" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G123" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="B124" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C124" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E124" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F124" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G124" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>44</v>
+      </c>
+      <c r="B125" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" t="s">
+        <v>13</v>
+      </c>
+      <c r="E125" t="s">
+        <v>14</v>
+      </c>
+      <c r="F125" t="s">
+        <v>15</v>
+      </c>
+      <c r="G125" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>97</v>
+      </c>
+      <c r="B126" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" t="s">
+        <v>13</v>
+      </c>
+      <c r="E126" t="s">
+        <v>14</v>
+      </c>
+      <c r="F126" t="s">
+        <v>15</v>
+      </c>
+      <c r="G126" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>45</v>
+      </c>
+      <c r="B127" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127" t="s">
+        <v>11</v>
+      </c>
+      <c r="D127" t="s">
+        <v>13</v>
+      </c>
+      <c r="E127" t="s">
+        <v>14</v>
+      </c>
+      <c r="F127" t="s">
+        <v>15</v>
+      </c>
+      <c r="G127" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>134</v>
+      </c>
+      <c r="B128" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128" t="s">
+        <v>20</v>
+      </c>
+      <c r="D128" t="s">
+        <v>16</v>
+      </c>
+      <c r="E128" t="s">
+        <v>17</v>
+      </c>
+      <c r="F128" t="s">
+        <v>18</v>
+      </c>
+      <c r="G128" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>46</v>
+      </c>
+      <c r="B129" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129" t="s">
+        <v>14</v>
+      </c>
+      <c r="F129" t="s">
+        <v>15</v>
+      </c>
+      <c r="G129" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>52</v>
+      </c>
+      <c r="B130" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" t="s">
+        <v>15</v>
+      </c>
+      <c r="G130" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>98</v>
+      </c>
+      <c r="B131" t="s">
+        <v>12</v>
+      </c>
+      <c r="C131" t="s">
+        <v>11</v>
+      </c>
+      <c r="D131" t="s">
+        <v>13</v>
+      </c>
+      <c r="E131" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131" t="s">
+        <v>15</v>
+      </c>
+      <c r="G131" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>164</v>
+      </c>
+      <c r="B132" t="s">
+        <v>12</v>
+      </c>
+      <c r="C132" t="s">
+        <v>11</v>
+      </c>
+      <c r="D132" t="s">
+        <v>13</v>
+      </c>
+      <c r="E132" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" t="s">
+        <v>15</v>
+      </c>
+      <c r="G132" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>47</v>
+      </c>
+      <c r="B133" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" t="s">
+        <v>11</v>
+      </c>
+      <c r="D133" t="s">
+        <v>13</v>
+      </c>
+      <c r="E133" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" t="s">
+        <v>15</v>
+      </c>
+      <c r="G133" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>166</v>
+      </c>
+      <c r="B134" t="s">
+        <v>12</v>
+      </c>
+      <c r="C134" t="s">
+        <v>11</v>
+      </c>
+      <c r="D134" t="s">
+        <v>13</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F134" t="s">
+        <v>15</v>
+      </c>
+      <c r="G134" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>165</v>
+      </c>
+      <c r="B135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135" t="s">
+        <v>11</v>
+      </c>
+      <c r="D135" t="s">
+        <v>13</v>
+      </c>
+      <c r="E135" t="s">
+        <v>14</v>
+      </c>
+      <c r="F135" t="s">
+        <v>15</v>
+      </c>
+      <c r="G135" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>48</v>
+      </c>
+      <c r="B136" t="s">
+        <v>12</v>
+      </c>
+      <c r="C136" t="s">
+        <v>11</v>
+      </c>
+      <c r="D136" t="s">
+        <v>13</v>
+      </c>
+      <c r="E136" t="s">
+        <v>14</v>
+      </c>
+      <c r="F136" t="s">
+        <v>15</v>
+      </c>
+      <c r="G136" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>104</v>
+      </c>
+      <c r="B137" t="s">
+        <v>12</v>
+      </c>
+      <c r="C137" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" t="s">
+        <v>20</v>
+      </c>
+      <c r="E137" t="s">
+        <v>14</v>
+      </c>
+      <c r="F137" t="s">
+        <v>12</v>
+      </c>
+      <c r="G137" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A124">
-    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
-    <cfRule type="notContainsText" dxfId="24" priority="17" operator="notContains" text=".igb">
+  <conditionalFormatting sqref="A2:A137">
+    <cfRule type="duplicateValues" dxfId="181" priority="16"/>
+    <cfRule type="notContainsText" dxfId="180" priority="17" operator="notContains" text=".igb">
       <formula>ISERROR(SEARCH(".igb",A2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B124">
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="notEqual">
+  <conditionalFormatting sqref="B2:B137">
+    <cfRule type="cellIs" dxfId="179" priority="10" operator="notEqual">
       <formula>"XML2 PC"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="12" operator="equal">
       <formula>"XML2 PC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F124">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Custom">
+  <conditionalFormatting sqref="B2:F137">
+    <cfRule type="containsText" dxfId="177" priority="1" operator="containsText" text="Custom">
       <formula>NOT(ISERROR(SEARCH("Custom",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C124">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="notEqual">
+  <conditionalFormatting sqref="C2:C137">
+    <cfRule type="cellIs" dxfId="176" priority="8" operator="notEqual">
       <formula>"XML2 GameCube"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="9" operator="equal">
       <formula>"XML2 GameCube"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D124">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="notEqual">
+  <conditionalFormatting sqref="D2:D137">
+    <cfRule type="cellIs" dxfId="174" priority="6" operator="notEqual">
       <formula>"XML2 PS2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="7" operator="equal">
       <formula>"XML2 PS2"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E124">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="notEqual">
+  <conditionalFormatting sqref="E2:E137">
+    <cfRule type="cellIs" dxfId="172" priority="4" operator="notEqual">
       <formula>"XML2 PSP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="5" operator="equal">
       <formula>"XML2 PSP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F124">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="notEqual">
+  <conditionalFormatting sqref="F2:F137">
+    <cfRule type="cellIs" dxfId="170" priority="2" operator="notEqual">
       <formula>"XML2 Xbox"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="3" operator="equal">
       <formula>"XML2 Xbox"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4054,13 +5952,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:F124</xm:sqref>
+          <xm:sqref>B2:F137</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2DF90B60-5089-44BA-BF59-8649B6D52DF3}">
           <x14:formula1>
             <xm:f>Sheet2!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G124</xm:sqref>
+          <xm:sqref>G2:G137</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Update Power Models and Textures.xlsx
</commit_message>
<xml_diff>
--- a/4. Menus/permanent/Power Models and Textures.xlsx
+++ b/4. Menus/permanent/Power Models and Textures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\XML2-Ultimate-Patch\4. Menus\permanent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC944D3-BA08-4106-9280-170798D33C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DFBAC4-A191-42AB-AF03-9689D3C130DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="168">
   <si>
     <t>File</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>textures\whiteflash.igb</t>
+  </si>
+  <si>
+    <t>textures\fog_jungle.igb</t>
   </si>
 </sst>
 </file>
@@ -585,1567 +588,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="182">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2420,10 +863,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G137" totalsRowShown="0">
-  <autoFilter ref="A1:G137" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G137">
-    <sortCondition ref="A1:A137"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G138" totalsRowShown="0">
+  <autoFilter ref="A1:G138" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G138">
+    <sortCondition ref="A1:A138"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6B176F19-9C3E-4D2F-9828-AA9A0F4398C8}" name="File"/>
@@ -2721,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3774,53 +2217,53 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G46" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F47" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G47" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -3838,12 +2281,12 @@
         <v>15</v>
       </c>
       <c r="G48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
@@ -3866,7 +2309,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
@@ -3889,7 +2332,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
@@ -3901,18 +2344,18 @@
         <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
       </c>
       <c r="G51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -3924,18 +2367,18 @@
         <v>13</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
       </c>
       <c r="G52" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
@@ -3958,7 +2401,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -3981,53 +2424,53 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D55" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E55" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G55" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G56" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
@@ -4039,18 +2482,18 @@
         <v>13</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
       </c>
       <c r="G57" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
         <v>12</v>
@@ -4073,168 +2516,168 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E59" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G59" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
         <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E60" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C61" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F61" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G61" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E62" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G62" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E63" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F63" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G63" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D64" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E64" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F64" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G64" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="B65" t="s">
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
@@ -4257,7 +2700,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
@@ -4269,18 +2712,18 @@
         <v>13</v>
       </c>
       <c r="E67" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F67" t="s">
         <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
@@ -4292,18 +2735,18 @@
         <v>13</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F68" t="s">
         <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
@@ -4321,12 +2764,12 @@
         <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
@@ -4349,7 +2792,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
@@ -4372,7 +2815,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
@@ -4395,7 +2838,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -4413,12 +2856,12 @@
         <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
         <v>12</v>
@@ -4436,58 +2879,58 @@
         <v>15</v>
       </c>
       <c r="G74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D75" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E75" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F75" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D76" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E76" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G76" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
@@ -4510,7 +2953,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
@@ -4528,12 +2971,12 @@
         <v>15</v>
       </c>
       <c r="G78" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
@@ -4551,12 +2994,12 @@
         <v>15</v>
       </c>
       <c r="G79" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
         <v>12</v>
@@ -4574,12 +3017,12 @@
         <v>15</v>
       </c>
       <c r="G80" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
@@ -4597,12 +3040,12 @@
         <v>15</v>
       </c>
       <c r="G81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
         <v>12</v>
@@ -4620,12 +3063,12 @@
         <v>15</v>
       </c>
       <c r="G82" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
@@ -4643,12 +3086,12 @@
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
@@ -4671,7 +3114,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
         <v>12</v>
@@ -4694,7 +3137,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
         <v>12</v>
@@ -4712,12 +3155,12 @@
         <v>15</v>
       </c>
       <c r="G86" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B87" t="s">
         <v>12</v>
@@ -4740,7 +3183,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B88" t="s">
         <v>12</v>
@@ -4758,12 +3201,12 @@
         <v>15</v>
       </c>
       <c r="G88" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>12</v>
@@ -4781,12 +3224,12 @@
         <v>15</v>
       </c>
       <c r="G89" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B90" t="s">
         <v>12</v>
@@ -4804,12 +3247,12 @@
         <v>15</v>
       </c>
       <c r="G90" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>12</v>
@@ -4827,35 +3270,35 @@
         <v>15</v>
       </c>
       <c r="G91" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D92" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E92" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F92" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G92" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B93" t="s">
         <v>21</v>
@@ -4878,99 +3321,99 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B94" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C94" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D94" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E94" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G94" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B95" t="s">
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D95" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E95" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G95" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D96" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
       </c>
       <c r="F96" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G96" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B97" t="s">
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D97" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
       </c>
       <c r="F97" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G97" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B98" t="s">
         <v>12</v>
@@ -4988,35 +3431,35 @@
         <v>15</v>
       </c>
       <c r="G98" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B99" t="s">
         <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D99" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
       </c>
       <c r="F99" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B100" t="s">
         <v>12</v>
@@ -5025,21 +3468,21 @@
         <v>20</v>
       </c>
       <c r="D100" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E100" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F100" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B101" t="s">
         <v>12</v>
@@ -5048,13 +3491,13 @@
         <v>20</v>
       </c>
       <c r="D101" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E101" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G101" t="s">
         <v>148</v>
@@ -5062,76 +3505,76 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="B102" t="s">
         <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D102" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E102" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F102" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G102" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="B103" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D103" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E103" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F103" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G103" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C104" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D104" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E104" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F104" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G104" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B105" t="s">
         <v>12</v>
@@ -5154,99 +3597,99 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D106" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E106" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F106" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G106" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D107" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E107" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F107" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G107" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D108" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E108" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F108" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G108" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="B109" t="s">
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D109" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E109" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F109" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G109" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
@@ -5264,35 +3707,35 @@
         <v>15</v>
       </c>
       <c r="G110" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>131</v>
+        <v>42</v>
       </c>
       <c r="B111" t="s">
         <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D111" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E111" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F111" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G111" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B112" t="s">
         <v>12</v>
@@ -5304,7 +3747,7 @@
         <v>20</v>
       </c>
       <c r="E112" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F112" t="s">
         <v>12</v>
@@ -5315,30 +3758,30 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="B113" t="s">
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D113" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E113" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F113" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G113" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
@@ -5350,18 +3793,18 @@
         <v>13</v>
       </c>
       <c r="E114" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F114" t="s">
         <v>15</v>
       </c>
       <c r="G114" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="B115" t="s">
         <v>12</v>
@@ -5379,12 +3822,12 @@
         <v>15</v>
       </c>
       <c r="G115" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="B116" t="s">
         <v>12</v>
@@ -5407,7 +3850,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B117" t="s">
         <v>12</v>
@@ -5430,7 +3873,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="B118" t="s">
         <v>12</v>
@@ -5453,7 +3896,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B119" t="s">
         <v>12</v>
@@ -5476,7 +3919,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
@@ -5499,122 +3942,122 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="B121" t="s">
         <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D121" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E121" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F121" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G121" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="B122" t="s">
         <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D122" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E122" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F122" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G122" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B123" t="s">
         <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D123" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E123" t="s">
         <v>14</v>
       </c>
       <c r="F123" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G123" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B124" t="s">
         <v>12</v>
       </c>
       <c r="C124" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E124" t="s">
         <v>14</v>
       </c>
       <c r="F124" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G124" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B125" t="s">
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D125" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E125" t="s">
         <v>14</v>
       </c>
       <c r="F125" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G125" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B126" t="s">
         <v>12</v>
@@ -5632,12 +4075,12 @@
         <v>15</v>
       </c>
       <c r="G126" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B127" t="s">
         <v>12</v>
@@ -5655,58 +4098,58 @@
         <v>15</v>
       </c>
       <c r="G127" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="B128" t="s">
         <v>12</v>
       </c>
       <c r="C128" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D128" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E128" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F128" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G128" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="B129" t="s">
         <v>12</v>
       </c>
       <c r="C129" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D129" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E129" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F129" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G129" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B130" t="s">
         <v>12</v>
@@ -5724,12 +4167,12 @@
         <v>15</v>
       </c>
       <c r="G130" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B131" t="s">
         <v>12</v>
@@ -5747,12 +4190,12 @@
         <v>15</v>
       </c>
       <c r="G131" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="B132" t="s">
         <v>12</v>
@@ -5775,7 +4218,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="B133" t="s">
         <v>12</v>
@@ -5793,12 +4236,12 @@
         <v>15</v>
       </c>
       <c r="G133" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>166</v>
+        <v>47</v>
       </c>
       <c r="B134" t="s">
         <v>12</v>
@@ -5816,12 +4259,12 @@
         <v>15</v>
       </c>
       <c r="G134" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B135" t="s">
         <v>12</v>
@@ -5844,7 +4287,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="B136" t="s">
         <v>12</v>
@@ -5862,82 +4305,105 @@
         <v>15</v>
       </c>
       <c r="G136" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>48</v>
+      </c>
+      <c r="B137" t="s">
+        <v>12</v>
+      </c>
+      <c r="C137" t="s">
+        <v>11</v>
+      </c>
+      <c r="D137" t="s">
+        <v>13</v>
+      </c>
+      <c r="E137" t="s">
+        <v>14</v>
+      </c>
+      <c r="F137" t="s">
+        <v>15</v>
+      </c>
+      <c r="G137" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>104</v>
       </c>
-      <c r="B137" t="s">
-        <v>12</v>
-      </c>
-      <c r="C137" t="s">
-        <v>20</v>
-      </c>
-      <c r="D137" t="s">
-        <v>20</v>
-      </c>
-      <c r="E137" t="s">
-        <v>14</v>
-      </c>
-      <c r="F137" t="s">
-        <v>12</v>
-      </c>
-      <c r="G137" t="s">
+      <c r="B138" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" t="s">
+        <v>20</v>
+      </c>
+      <c r="D138" t="s">
+        <v>20</v>
+      </c>
+      <c r="E138" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138" t="s">
+        <v>12</v>
+      </c>
+      <c r="G138" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A137">
-    <cfRule type="duplicateValues" dxfId="181" priority="16"/>
-    <cfRule type="notContainsText" dxfId="180" priority="17" operator="notContains" text=".igb">
+  <conditionalFormatting sqref="A2:A138">
+    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
+    <cfRule type="notContainsText" dxfId="24" priority="17" operator="notContains" text=".igb">
       <formula>ISERROR(SEARCH(".igb",A2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B137">
-    <cfRule type="cellIs" dxfId="179" priority="10" operator="notEqual">
+  <conditionalFormatting sqref="B2:B138">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="notEqual">
       <formula>"XML2 PC"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
       <formula>"XML2 PC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F137">
-    <cfRule type="containsText" dxfId="177" priority="1" operator="containsText" text="Custom">
+  <conditionalFormatting sqref="B2:F138">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Custom">
       <formula>NOT(ISERROR(SEARCH("Custom",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C137">
-    <cfRule type="cellIs" dxfId="176" priority="8" operator="notEqual">
+  <conditionalFormatting sqref="C2:C138">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="notEqual">
       <formula>"XML2 GameCube"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"XML2 GameCube"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D137">
-    <cfRule type="cellIs" dxfId="174" priority="6" operator="notEqual">
+  <conditionalFormatting sqref="D2:D138">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="notEqual">
       <formula>"XML2 PS2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"XML2 PS2"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E137">
-    <cfRule type="cellIs" dxfId="172" priority="4" operator="notEqual">
+  <conditionalFormatting sqref="E2:E138">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="notEqual">
       <formula>"XML2 PSP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"XML2 PSP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F137">
-    <cfRule type="cellIs" dxfId="170" priority="2" operator="notEqual">
+  <conditionalFormatting sqref="F2:F138">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="notEqual">
       <formula>"XML2 Xbox"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"XML2 Xbox"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5952,13 +4418,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:F137</xm:sqref>
+          <xm:sqref>B2:F138</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2DF90B60-5089-44BA-BF59-8649B6D52DF3}">
           <x14:formula1>
             <xm:f>Sheet2!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G137</xm:sqref>
+          <xm:sqref>G2:G138</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
bolt_softedge: Add source information
</commit_message>
<xml_diff>
--- a/4. Menus/permanent/Power Models and Textures.xlsx
+++ b/4. Menus/permanent/Power Models and Textures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\XML2-Ultimate-Patch\4. Menus\permanent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DFBAC4-A191-42AB-AF03-9689D3C130DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620B0AAE-9CC2-4CD6-A9E3-4A4CA5C57BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="169">
   <si>
     <t>File</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>textures\fog_jungle.igb</t>
+  </si>
+  <si>
+    <t>textures\bolt_softedge.igb</t>
   </si>
 </sst>
 </file>
@@ -863,10 +866,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G138" totalsRowShown="0">
-  <autoFilter ref="A1:G138" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G138">
-    <sortCondition ref="A1:A138"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}" name="Table2" displayName="Table2" ref="A1:G139" totalsRowShown="0">
+  <autoFilter ref="A1:G139" xr:uid="{BFB36695-8DBB-4824-8420-18F9B34B1C91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G139">
+    <sortCondition ref="A1:A139"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6B176F19-9C3E-4D2F-9828-AA9A0F4398C8}" name="File"/>
@@ -1164,18 +1167,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G138"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="2" max="6" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="78.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1665,10 +1666,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -1677,41 +1678,41 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
@@ -1734,7 +1735,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
@@ -1757,7 +1758,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -1780,7 +1781,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -1803,7 +1804,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -1826,7 +1827,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
@@ -1849,7 +1850,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -1872,7 +1873,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
@@ -1895,7 +1896,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -1918,7 +1919,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -1941,7 +1942,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -1959,58 +1960,58 @@
         <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
         <v>21</v>
@@ -2033,7 +2034,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
         <v>21</v>
@@ -2056,30 +2057,30 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G39" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
@@ -2097,81 +2098,81 @@
         <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F41" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G42" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
@@ -2194,99 +2195,99 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G45" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G46" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F47" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G48" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
@@ -2304,12 +2305,12 @@
         <v>15</v>
       </c>
       <c r="G49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
@@ -2332,7 +2333,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
@@ -2355,7 +2356,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -2367,18 +2368,18 @@
         <v>13</v>
       </c>
       <c r="E52" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
       </c>
       <c r="G52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
@@ -2390,18 +2391,18 @@
         <v>13</v>
       </c>
       <c r="E53" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
       </c>
       <c r="G53" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2424,7 +2425,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -2447,53 +2448,53 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D56" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
         <v>12</v>
@@ -2505,18 +2506,18 @@
         <v>13</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
       </c>
       <c r="G58" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
@@ -2539,168 +2540,168 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E61" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G61" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G62" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E63" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G63" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F64" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D65" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E65" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G65" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G66" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
@@ -2723,7 +2724,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
@@ -2735,18 +2736,18 @@
         <v>13</v>
       </c>
       <c r="E68" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F68" t="s">
         <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
@@ -2758,18 +2759,18 @@
         <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F69" t="s">
         <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
@@ -2787,12 +2788,12 @@
         <v>15</v>
       </c>
       <c r="G70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
@@ -2815,7 +2816,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
@@ -2838,7 +2839,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -2861,7 +2862,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
         <v>12</v>
@@ -2879,12 +2880,12 @@
         <v>15</v>
       </c>
       <c r="G74" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
@@ -2902,58 +2903,58 @@
         <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E76" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G76" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D77" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E77" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
@@ -2976,7 +2977,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
@@ -2994,12 +2995,12 @@
         <v>15</v>
       </c>
       <c r="G79" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="B80" t="s">
         <v>12</v>
@@ -3017,12 +3018,12 @@
         <v>15</v>
       </c>
       <c r="G80" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
@@ -3040,12 +3041,12 @@
         <v>15</v>
       </c>
       <c r="G81" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B82" t="s">
         <v>12</v>
@@ -3063,12 +3064,12 @@
         <v>15</v>
       </c>
       <c r="G82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
@@ -3086,12 +3087,12 @@
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
@@ -3109,12 +3110,12 @@
         <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
         <v>12</v>
@@ -3137,7 +3138,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
         <v>12</v>
@@ -3160,7 +3161,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
         <v>12</v>
@@ -3178,12 +3179,12 @@
         <v>15</v>
       </c>
       <c r="G87" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B88" t="s">
         <v>12</v>
@@ -3206,7 +3207,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B89" t="s">
         <v>12</v>
@@ -3224,12 +3225,12 @@
         <v>15</v>
       </c>
       <c r="G89" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>12</v>
@@ -3247,12 +3248,12 @@
         <v>15</v>
       </c>
       <c r="G90" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B91" t="s">
         <v>12</v>
@@ -3270,12 +3271,12 @@
         <v>15</v>
       </c>
       <c r="G91" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
         <v>12</v>
@@ -3293,35 +3294,35 @@
         <v>15</v>
       </c>
       <c r="G92" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D93" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E93" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F93" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G93" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
         <v>21</v>
@@ -3344,99 +3345,99 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C95" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D95" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E95" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G95" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D96" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E96" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G96" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B97" t="s">
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
       </c>
       <c r="F97" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G97" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B98" t="s">
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
       </c>
       <c r="F98" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G98" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B99" t="s">
         <v>12</v>
@@ -3454,35 +3455,35 @@
         <v>15</v>
       </c>
       <c r="G99" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B100" t="s">
         <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D100" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E100" t="s">
         <v>14</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B101" t="s">
         <v>12</v>
@@ -3491,21 +3492,21 @@
         <v>20</v>
       </c>
       <c r="D101" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E101" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F101" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B102" t="s">
         <v>12</v>
@@ -3514,13 +3515,13 @@
         <v>20</v>
       </c>
       <c r="D102" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E102" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F102" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G102" t="s">
         <v>148</v>
@@ -3528,76 +3529,76 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="B103" t="s">
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E103" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F103" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G103" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="B104" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D104" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E104" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F104" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G104" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C105" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D105" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E105" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F105" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G105" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
@@ -3620,99 +3621,99 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D107" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E107" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F107" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G107" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D108" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E108" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F108" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G108" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="B109" t="s">
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D109" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E109" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F109" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G109" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D110" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E110" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F110" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G110" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B111" t="s">
         <v>12</v>
@@ -3730,35 +3731,35 @@
         <v>15</v>
       </c>
       <c r="G111" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>131</v>
+        <v>42</v>
       </c>
       <c r="B112" t="s">
         <v>12</v>
       </c>
       <c r="C112" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D112" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E112" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F112" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G112" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B113" t="s">
         <v>12</v>
@@ -3770,7 +3771,7 @@
         <v>20</v>
       </c>
       <c r="E113" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F113" t="s">
         <v>12</v>
@@ -3781,30 +3782,30 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D114" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E114" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F114" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G114" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="B115" t="s">
         <v>12</v>
@@ -3816,18 +3817,18 @@
         <v>13</v>
       </c>
       <c r="E115" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F115" t="s">
         <v>15</v>
       </c>
       <c r="G115" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="B116" t="s">
         <v>12</v>
@@ -3845,12 +3846,12 @@
         <v>15</v>
       </c>
       <c r="G116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="B117" t="s">
         <v>12</v>
@@ -3873,7 +3874,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B118" t="s">
         <v>12</v>
@@ -3896,7 +3897,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="B119" t="s">
         <v>12</v>
@@ -3919,7 +3920,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
@@ -3942,7 +3943,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B121" t="s">
         <v>12</v>
@@ -3965,122 +3966,122 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="B122" t="s">
         <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D122" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E122" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F122" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G122" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="B123" t="s">
         <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D123" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E123" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F123" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G123" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B124" t="s">
         <v>12</v>
       </c>
       <c r="C124" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E124" t="s">
         <v>14</v>
       </c>
       <c r="F124" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G124" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B125" t="s">
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E125" t="s">
         <v>14</v>
       </c>
       <c r="F125" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G125" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B126" t="s">
         <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D126" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E126" t="s">
         <v>14</v>
       </c>
       <c r="F126" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G126" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B127" t="s">
         <v>12</v>
@@ -4098,12 +4099,12 @@
         <v>15</v>
       </c>
       <c r="G127" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B128" t="s">
         <v>12</v>
@@ -4121,58 +4122,58 @@
         <v>15</v>
       </c>
       <c r="G128" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="B129" t="s">
         <v>12</v>
       </c>
       <c r="C129" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D129" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E129" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F129" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G129" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="B130" t="s">
         <v>12</v>
       </c>
       <c r="C130" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D130" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E130" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F130" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G130" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B131" t="s">
         <v>12</v>
@@ -4190,12 +4191,12 @@
         <v>15</v>
       </c>
       <c r="G131" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B132" t="s">
         <v>12</v>
@@ -4213,12 +4214,12 @@
         <v>15</v>
       </c>
       <c r="G132" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="B133" t="s">
         <v>12</v>
@@ -4241,7 +4242,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="B134" t="s">
         <v>12</v>
@@ -4259,12 +4260,12 @@
         <v>15</v>
       </c>
       <c r="G134" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>166</v>
+        <v>47</v>
       </c>
       <c r="B135" t="s">
         <v>12</v>
@@ -4282,12 +4283,12 @@
         <v>15</v>
       </c>
       <c r="G135" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B136" t="s">
         <v>12</v>
@@ -4310,7 +4311,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="B137" t="s">
         <v>12</v>
@@ -4328,41 +4329,64 @@
         <v>15</v>
       </c>
       <c r="G137" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>48</v>
+      </c>
+      <c r="B138" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" t="s">
+        <v>11</v>
+      </c>
+      <c r="D138" t="s">
+        <v>13</v>
+      </c>
+      <c r="E138" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138" t="s">
+        <v>15</v>
+      </c>
+      <c r="G138" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>104</v>
       </c>
-      <c r="B138" t="s">
-        <v>12</v>
-      </c>
-      <c r="C138" t="s">
-        <v>20</v>
-      </c>
-      <c r="D138" t="s">
-        <v>20</v>
-      </c>
-      <c r="E138" t="s">
-        <v>14</v>
-      </c>
-      <c r="F138" t="s">
-        <v>12</v>
-      </c>
-      <c r="G138" t="s">
+      <c r="B139" t="s">
+        <v>12</v>
+      </c>
+      <c r="C139" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139" t="s">
+        <v>20</v>
+      </c>
+      <c r="E139" t="s">
+        <v>14</v>
+      </c>
+      <c r="F139" t="s">
+        <v>12</v>
+      </c>
+      <c r="G139" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A138">
+  <conditionalFormatting sqref="A2:A139">
     <cfRule type="duplicateValues" dxfId="25" priority="16"/>
     <cfRule type="notContainsText" dxfId="24" priority="17" operator="notContains" text=".igb">
       <formula>ISERROR(SEARCH(".igb",A2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B138">
+  <conditionalFormatting sqref="B2:B139">
     <cfRule type="cellIs" dxfId="23" priority="10" operator="notEqual">
       <formula>"XML2 PC"</formula>
     </cfRule>
@@ -4370,12 +4394,12 @@
       <formula>"XML2 PC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F138">
+  <conditionalFormatting sqref="B2:F139">
     <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Custom">
       <formula>NOT(ISERROR(SEARCH("Custom",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C138">
+  <conditionalFormatting sqref="C2:C139">
     <cfRule type="cellIs" dxfId="20" priority="8" operator="notEqual">
       <formula>"XML2 GameCube"</formula>
     </cfRule>
@@ -4383,7 +4407,7 @@
       <formula>"XML2 GameCube"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D138">
+  <conditionalFormatting sqref="D2:D139">
     <cfRule type="cellIs" dxfId="18" priority="6" operator="notEqual">
       <formula>"XML2 PS2"</formula>
     </cfRule>
@@ -4391,7 +4415,7 @@
       <formula>"XML2 PS2"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E138">
+  <conditionalFormatting sqref="E2:E139">
     <cfRule type="cellIs" dxfId="16" priority="4" operator="notEqual">
       <formula>"XML2 PSP"</formula>
     </cfRule>
@@ -4399,7 +4423,7 @@
       <formula>"XML2 PSP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F138">
+  <conditionalFormatting sqref="F2:F139">
     <cfRule type="cellIs" dxfId="14" priority="2" operator="notEqual">
       <formula>"XML2 Xbox"</formula>
     </cfRule>
@@ -4418,13 +4442,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:F138</xm:sqref>
+          <xm:sqref>B2:F139</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2DF90B60-5089-44BA-BF59-8649B6D52DF3}">
           <x14:formula1>
             <xm:f>Sheet2!$C$2:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G138</xm:sqref>
+          <xm:sqref>G2:G139</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>